<commit_message>
fix some cetasika naming
</commit_message>
<xml_diff>
--- a/documents/Sheet.xlsx
+++ b/documents/Sheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jordi\Home\20_Areas\10_Dhammobhasa\dhammo-konvajs\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E49625-27A9-4E52-B5CA-BC6BB37AA8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0EA213-D854-435C-8D36-1F05599A2BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18150" yWindow="-11160" windowWidth="17895" windowHeight="10545" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Citta" sheetId="1" r:id="rId1"/>
     <sheet name="Citta layout" sheetId="2" r:id="rId2"/>
     <sheet name="Cetasika" sheetId="3" r:id="rId3"/>
+    <sheet name="Cetasika layout" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="233">
   <si>
     <t>id</t>
   </si>
@@ -459,6 +460,273 @@
   </si>
   <si>
     <t>group</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phassa</t>
+  </si>
+  <si>
+    <t>sanna</t>
+  </si>
+  <si>
+    <t>cetana</t>
+  </si>
+  <si>
+    <t>ekaggata</t>
+  </si>
+  <si>
+    <t>jivitindriya</t>
+  </si>
+  <si>
+    <t>manasikara</t>
+  </si>
+  <si>
+    <t>vitakka</t>
+  </si>
+  <si>
+    <t>vicara</t>
+  </si>
+  <si>
+    <t>adhimokha</t>
+  </si>
+  <si>
+    <t>viriya</t>
+  </si>
+  <si>
+    <t>piti</t>
+  </si>
+  <si>
+    <t>chanda</t>
+  </si>
+  <si>
+    <t>ahirika</t>
+  </si>
+  <si>
+    <t>anottappa</t>
+  </si>
+  <si>
+    <t>uddaccha</t>
+  </si>
+  <si>
+    <t>ditthi</t>
+  </si>
+  <si>
+    <t>mana</t>
+  </si>
+  <si>
+    <t>issa</t>
+  </si>
+  <si>
+    <t>macchariya</t>
+  </si>
+  <si>
+    <t>kukuccha</t>
+  </si>
+  <si>
+    <t>thina</t>
+  </si>
+  <si>
+    <t>middha</t>
+  </si>
+  <si>
+    <t>vicikiccha</t>
+  </si>
+  <si>
+    <t>saddha</t>
+  </si>
+  <si>
+    <t>sati</t>
+  </si>
+  <si>
+    <t>hiri</t>
+  </si>
+  <si>
+    <t>ottappa</t>
+  </si>
+  <si>
+    <t>alobha</t>
+  </si>
+  <si>
+    <t>adosa</t>
+  </si>
+  <si>
+    <t>tatramajjhattata</t>
+  </si>
+  <si>
+    <t>kayapasadhi</t>
+  </si>
+  <si>
+    <t>kayalahutta</t>
+  </si>
+  <si>
+    <t>kayamudutta</t>
+  </si>
+  <si>
+    <t>kayakammannata</t>
+  </si>
+  <si>
+    <t>kayapagunnata</t>
+  </si>
+  <si>
+    <t>kayujukata</t>
+  </si>
+  <si>
+    <t>cittapasadhi</t>
+  </si>
+  <si>
+    <t>cittalahutta</t>
+  </si>
+  <si>
+    <t>cittamudutta</t>
+  </si>
+  <si>
+    <t>cittakammannata</t>
+  </si>
+  <si>
+    <t>cittapagunnata</t>
+  </si>
+  <si>
+    <t>cittujukata</t>
+  </si>
+  <si>
+    <t>sammavaca</t>
+  </si>
+  <si>
+    <t>sammakammanta</t>
+  </si>
+  <si>
+    <t>sammajiva</t>
+  </si>
+  <si>
+    <t>karuna</t>
+  </si>
+  <si>
+    <t>mudita</t>
+  </si>
+  <si>
+    <t>panna</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>vedanā</t>
+  </si>
+  <si>
+    <t>issā</t>
+  </si>
+  <si>
+    <t>saññā</t>
+  </si>
+  <si>
+    <t>cetanā</t>
+  </si>
+  <si>
+    <t>ekaggatā</t>
+  </si>
+  <si>
+    <t>jīvitindriya</t>
+  </si>
+  <si>
+    <t>manasikāra</t>
+  </si>
+  <si>
+    <t>vicāra</t>
+  </si>
+  <si>
+    <t>adhimokkha</t>
+  </si>
+  <si>
+    <t>vīriya</t>
+  </si>
+  <si>
+    <t>pīti</t>
+  </si>
+  <si>
+    <t>uddhacca</t>
+  </si>
+  <si>
+    <t>diṭṭhi</t>
+  </si>
+  <si>
+    <t>māna</t>
+  </si>
+  <si>
+    <t>kukkucca</t>
+  </si>
+  <si>
+    <t>vicikicchā</t>
+  </si>
+  <si>
+    <t>saddhā</t>
+  </si>
+  <si>
+    <t>hirī</t>
+  </si>
+  <si>
+    <t>tatramajjhattatā</t>
+  </si>
+  <si>
+    <t>kāyapassaddhi</t>
+  </si>
+  <si>
+    <t>cittapassaddhi</t>
+  </si>
+  <si>
+    <t>kāyalahutā</t>
+  </si>
+  <si>
+    <t>cittalahutā</t>
+  </si>
+  <si>
+    <t>kāyamudutā</t>
+  </si>
+  <si>
+    <t>cittamudutā</t>
+  </si>
+  <si>
+    <t>kāyakammaññatā</t>
+  </si>
+  <si>
+    <t>cittakammaññatā</t>
+  </si>
+  <si>
+    <t>kāyapāguññatā</t>
+  </si>
+  <si>
+    <t>cittapāguññatā</t>
+  </si>
+  <si>
+    <t>kāyujukatā</t>
+  </si>
+  <si>
+    <t>cittujukatā</t>
+  </si>
+  <si>
+    <t>sammāvācā</t>
+  </si>
+  <si>
+    <t>sammākammanta</t>
+  </si>
+  <si>
+    <t>sammāājīva</t>
+  </si>
+  <si>
+    <t>karuṇā</t>
+  </si>
+  <si>
+    <t>muditā</t>
+  </si>
+  <si>
+    <t>paññā</t>
+  </si>
+  <si>
+    <t>hetu</t>
+  </si>
+  <si>
+    <t>amoha</t>
   </si>
 </sst>
 </file>
@@ -820,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30282B-4D63-4407-A836-371A28DA1D49}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="155" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A122"/>
+    <sheetView zoomScale="155" workbookViewId="0">
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2916,7 +3184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA613E0A-9705-48A8-9748-B384556521F6}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
@@ -4637,14 +4905,1544 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DC72FF-BEDA-4115-96FD-61449208A603}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E53" sqref="A1:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>208</v>
+      </c>
+      <c r="D25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>210</v>
+      </c>
+      <c r="D29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>212</v>
+      </c>
+      <c r="D35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>213</v>
+      </c>
+      <c r="D36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>215</v>
+      </c>
+      <c r="D37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>217</v>
+      </c>
+      <c r="D38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>219</v>
+      </c>
+      <c r="D39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>179</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>223</v>
+      </c>
+      <c r="D41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>214</v>
+      </c>
+      <c r="D42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>216</v>
+      </c>
+      <c r="D43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>218</v>
+      </c>
+      <c r="D44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>184</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>220</v>
+      </c>
+      <c r="D45" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>222</v>
+      </c>
+      <c r="D46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>225</v>
+      </c>
+      <c r="D48" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>188</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>226</v>
+      </c>
+      <c r="D49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>189</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>227</v>
+      </c>
+      <c r="D50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>228</v>
+      </c>
+      <c r="D51" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
+        <v>229</v>
+      </c>
+      <c r="D52" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>230</v>
+      </c>
+      <c r="D53" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2492DB43-9378-45F2-AB43-5650E18B2CF8}">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D53" sqref="A1:D53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>179</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>184</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>188</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>189</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add state management
</commit_message>
<xml_diff>
--- a/documents/Sheet.xlsx
+++ b/documents/Sheet.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jordi\Home\20_Areas\10_Dhammobhasa\dhammo-konvajs\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0EA213-D854-435C-8D36-1F05599A2BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3F360D-F059-4288-9030-1662A8B2D53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Citta" sheetId="1" r:id="rId1"/>
     <sheet name="Citta layout" sheetId="2" r:id="rId2"/>
     <sheet name="Cetasika" sheetId="3" r:id="rId3"/>
     <sheet name="Cetasika layout" sheetId="4" r:id="rId4"/>
+    <sheet name="Cittuppada" sheetId="5" r:id="rId5"/>
+    <sheet name="Cetasika groups" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="260">
   <si>
     <t>id</t>
   </si>
@@ -727,6 +729,87 @@
   </si>
   <si>
     <t>amoha</t>
+  </si>
+  <si>
+    <t>cittaId</t>
+  </si>
+  <si>
+    <t>always</t>
+  </si>
+  <si>
+    <t>groupId</t>
+  </si>
+  <si>
+    <t>cetasika/1</t>
+  </si>
+  <si>
+    <t>cetasika/2</t>
+  </si>
+  <si>
+    <t>cetasika/3</t>
+  </si>
+  <si>
+    <t>cetasika/4</t>
+  </si>
+  <si>
+    <t>cetasika/5</t>
+  </si>
+  <si>
+    <t>cetasika/6</t>
+  </si>
+  <si>
+    <t>cetasika/7</t>
+  </si>
+  <si>
+    <t>cetasika/8</t>
+  </si>
+  <si>
+    <t>cetasika/9</t>
+  </si>
+  <si>
+    <t>cetasika/10</t>
+  </si>
+  <si>
+    <t>cetasika/11</t>
+  </si>
+  <si>
+    <t>cetasika/12</t>
+  </si>
+  <si>
+    <t>cetasika/13</t>
+  </si>
+  <si>
+    <t>cetasika/14</t>
+  </si>
+  <si>
+    <t>cetasika/15</t>
+  </si>
+  <si>
+    <t>cetasika/16</t>
+  </si>
+  <si>
+    <t>cetasika/17</t>
+  </si>
+  <si>
+    <t>cetasika/18</t>
+  </si>
+  <si>
+    <t>cetasika/19</t>
+  </si>
+  <si>
+    <t>anottapa</t>
+  </si>
+  <si>
+    <t>universal</t>
+  </si>
+  <si>
+    <t>sobhana</t>
+  </si>
+  <si>
+    <t>virati</t>
+  </si>
+  <si>
+    <t>sammaajiva</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1172,7 @@
   <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView zoomScale="155" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+      <selection activeCell="A122" sqref="A2:A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4907,8 +4990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DC72FF-BEDA-4115-96FD-61449208A603}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E53" sqref="A1:E53"/>
+    <sheetView topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5692,7 +5775,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D53" sqref="A1:D53"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6445,4 +6528,868 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFAFA38-A549-4DFB-AF75-9F713BE94DA0}">
+  <dimension ref="A1:B122"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11AFBC05-20B7-4C67-B971-1B13AF228B2C}">
+  <dimension ref="A1:T33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="20" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1" t="s">
+        <v>243</v>
+      </c>
+      <c r="J1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K1" t="s">
+        <v>245</v>
+      </c>
+      <c r="L1" t="s">
+        <v>246</v>
+      </c>
+      <c r="M1" t="s">
+        <v>247</v>
+      </c>
+      <c r="N1" t="s">
+        <v>248</v>
+      </c>
+      <c r="O1" t="s">
+        <v>249</v>
+      </c>
+      <c r="P1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>251</v>
+      </c>
+      <c r="R1" t="s">
+        <v>252</v>
+      </c>
+      <c r="S1" t="s">
+        <v>253</v>
+      </c>
+      <c r="T1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" xr:uid="{94933E23-3390-4A61-B502-094C1636279A}">
+          <x14:formula1>
+            <xm:f>Cetasika!$A$2:$A$53</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:T20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add citta name
</commit_message>
<xml_diff>
--- a/documents/Sheet.xlsx
+++ b/documents/Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jordi\Home\20_Areas\10_Dhammobhasa\dhammo-konvajs\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3F360D-F059-4288-9030-1662A8B2D53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45E4847-B20D-44A3-A70C-AA3B39E607AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Citta" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="381">
   <si>
     <t>id</t>
   </si>
@@ -810,6 +810,369 @@
   </si>
   <si>
     <t>sammaajiva</t>
+  </si>
+  <si>
+    <t>somanassasahagata diṭṭhigatasampayutta asaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata diṭṭhigatavippayutta asaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata diṭṭhigatasampayutta sasaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata diṭṭhigatavippayutta sasaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata diṭṭhigatasampayutta asaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata diṭṭhigatasampayutta sasaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata diṭṭhigatavippayutta asaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata diṭṭhigatavippayutta sasaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇasampayutta asaṅkhārika kusala citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇasampayutta sasaṅkhārika kusala citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇavippayutta asaṅkhārika kusala citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇavippayutta sasaṅkhārika kusala citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇasampayutta asaṅkhārika kusala citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇasampayutta sasaṅkhārika kusala citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇavippayutta asaṅkhārika kusala citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇavippayutta sasaṅkhārika kusala citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇasampayutta asaṅkhārika vipāka citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇasampayutta sasaṅkhārika vipāka citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇavippayutta asaṅkhārika vipāka citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇavippayutta sasaṅkhārika vipāka citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇasampayutta asaṅkhārika vipāka citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇasampayutta sasaṅkhārika vipāka citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇavippayutta asaṅkhārika vipāka citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇavippayutta sasaṅkhārika vipāka citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇasampayutta asaṅkhārika kiriya citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇasampayutta sasaṅkhārika kiriya citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇavippayutta asaṅkhārika kiriya citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata ñāṇavippayutta sasaṅkhārika kiriya citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇasampayutta asaṅkhārika kiriya citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇasampayutta sasaṅkhārika kiriya citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇavippayutta asaṅkhārika kiriya citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata ñāṇavippayutta sasaṅkhārika kiriya citta</t>
+  </si>
+  <si>
+    <t>domanassasahagata paṭighasampayutta asaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>domanassasahagata paṭighasampayutta sasaṅkhārika citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata uddhacchasampayutta citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata vicikicchāsampayutta citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata akusalavipāka cakkhuviññāṇa</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata akusalavipāka sotaviññāṇa</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata akusalavipāka ghānaviññāṇa</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata akusalavipāka jivhāviññāṇa</t>
+  </si>
+  <si>
+    <t>dukkhasahagata akusalavipāka kāyaviññāṇa</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata akusalavipāka sampaṭicchana citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata akusalavipāka santīraṇa citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata kusalavipāka cakkhuviññāṇa</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata kusalavipāka sotaviññāṇa</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata kusalavipāka ghānaviññāṇa</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata kusalavipāka jivhāviññāṇa</t>
+  </si>
+  <si>
+    <t>sukhasahagata kusalavipāka kāyaviññāṇa</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata kusalavipāka sampaṭicchana citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata kusalavipāka santīraṇa citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata kusalavipāka santīraṇa citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata pañcadvārāvajjana citta</t>
+  </si>
+  <si>
+    <t>upekkhāsahagata manodvārāvajjanacitta citta</t>
+  </si>
+  <si>
+    <t>somanassasahagata hasituppāda citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhāna sotāpattimagga citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhāna sotāpattimagga citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhāna sotāpattimagga citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhāna sotāpattimagga citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhāna sotāpattimagga citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhāna sakadāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhāna sakadāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhāna sakadāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhāna sakadāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhāna sakadāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhāna anāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhāna anāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhāna anāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhāna anāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhāna anāgāmimagga citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhāna arahattamagga citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhāna arahattamagga citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhāna arahattamagga citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhāna arahattamagga citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhāna arahattamagga citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhāna sotāpattiphala citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhāna sotāpattiphala citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhāna sotāpattiphala citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhāna sotāpattiphala citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhāna sotāpattiphala citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhāna sakadāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhāna sakadāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhāna sakadāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhāna sakadāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhāna sakadāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhāna anāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhāna anāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhāna anāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhāna anāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhāna anāgāmiphala citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhāna arahattaphala citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhāna arahattaphala citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhāna arahattaphala citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhāna arahattaphala citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhāna arahattaphala citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhānakusala citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhānakusala citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhānakusala citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhānakusala citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhānakusala citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhānavipāka citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhānavipāka citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhānavipāka citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhānavipāka citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhānavipāka citta</t>
+  </si>
+  <si>
+    <t>vitakkavicārapītisukhekaggatāsahita paṭhamajjhānakiriya citta</t>
+  </si>
+  <si>
+    <t>vicārapītisukhekaggatāsahita dutiyajjhānakiriya citta</t>
+  </si>
+  <si>
+    <t>pītisukhekaggatāsahita tatiyajjhānakiriya citta</t>
+  </si>
+  <si>
+    <t>sukhekaggatāsahita catutthajjhānakiriya citta</t>
+  </si>
+  <si>
+    <t>upekkhekaggatāsahita pañcamajjhānakiriya citta</t>
+  </si>
+  <si>
+    <t>ākāsānañcāyatana kusala citta</t>
+  </si>
+  <si>
+    <t>viññāṇañcāyatana kusala citta</t>
+  </si>
+  <si>
+    <t>ākiñcaññāyatana kusala citta</t>
+  </si>
+  <si>
+    <t>nevasaññānāsaññāyatana kusala citta</t>
+  </si>
+  <si>
+    <t>ākāsānañcāyatana vipāka citta</t>
+  </si>
+  <si>
+    <t>viññāṇañcāyatana vipāka citta</t>
+  </si>
+  <si>
+    <t>ākiñcaññāyatana vipāka citta</t>
+  </si>
+  <si>
+    <t>nevasaññānāsaññāyatana vipāka citta</t>
+  </si>
+  <si>
+    <t>ākāsānañcāyatana kiriya citta</t>
+  </si>
+  <si>
+    <t>viññāṇañcāyatana kiriya citta</t>
+  </si>
+  <si>
+    <t>ākiñcaññāyatana kiriya citta</t>
+  </si>
+  <si>
+    <t>nevasaññānāsaññāyatana kiriya citta</t>
   </si>
 </sst>
 </file>
@@ -1169,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30282B-4D63-4407-A836-371A28DA1D49}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView zoomScale="155" workbookViewId="0">
-      <selection activeCell="A122" sqref="A2:A122"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,9 +1544,10 @@
     <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1199,8 +1563,11 @@
       <c r="E1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1216,8 +1583,11 @@
       <c r="E2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1233,8 +1603,11 @@
       <c r="E3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1250,8 +1623,11 @@
       <c r="E4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1267,8 +1643,11 @@
       <c r="E5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1284,8 +1663,11 @@
       <c r="E6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1301,8 +1683,11 @@
       <c r="E7" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1318,8 +1703,11 @@
       <c r="E8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1335,8 +1723,11 @@
       <c r="E9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1352,8 +1743,11 @@
       <c r="E10" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1369,8 +1763,11 @@
       <c r="E11" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1386,8 +1783,11 @@
       <c r="E12" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1403,8 +1803,11 @@
       <c r="E13" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1420,8 +1823,11 @@
       <c r="E14" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1437,8 +1843,11 @@
       <c r="E15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1454,8 +1863,11 @@
       <c r="E16" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1471,8 +1883,11 @@
       <c r="E17" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1488,8 +1903,11 @@
       <c r="E18" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -1505,8 +1923,11 @@
       <c r="E19" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -1522,8 +1943,11 @@
       <c r="E20" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1539,8 +1963,11 @@
       <c r="E21" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1556,8 +1983,11 @@
       <c r="E22" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1573,8 +2003,11 @@
       <c r="E23" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1590,8 +2023,11 @@
       <c r="E24" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1607,8 +2043,11 @@
       <c r="E25" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -1624,8 +2063,11 @@
       <c r="E26" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>118</v>
       </c>
@@ -1641,8 +2083,11 @@
       <c r="E27" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -1658,8 +2103,11 @@
       <c r="E28" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -1675,8 +2123,11 @@
       <c r="E29" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -1692,8 +2143,11 @@
       <c r="E30" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -1709,8 +2163,11 @@
       <c r="E31" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -1726,8 +2183,11 @@
       <c r="E32" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1743,8 +2203,11 @@
       <c r="E33" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1760,8 +2223,11 @@
       <c r="E34" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1777,8 +2243,11 @@
       <c r="E35" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1794,8 +2263,11 @@
       <c r="E36" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1811,8 +2283,11 @@
       <c r="E37" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -1828,8 +2303,11 @@
       <c r="E38" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1845,8 +2323,11 @@
       <c r="E39" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1862,8 +2343,11 @@
       <c r="E40" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -1879,8 +2363,11 @@
       <c r="E41" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -1896,8 +2383,11 @@
       <c r="E42" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -1913,8 +2403,11 @@
       <c r="E43" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -1930,8 +2423,11 @@
       <c r="E44" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -1947,8 +2443,11 @@
       <c r="E45" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>37</v>
       </c>
@@ -1964,8 +2463,11 @@
       <c r="E46" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -1981,8 +2483,11 @@
       <c r="E47" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1998,8 +2503,11 @@
       <c r="E48" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -2015,8 +2523,11 @@
       <c r="E49" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -2032,8 +2543,11 @@
       <c r="E50" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -2049,8 +2563,11 @@
       <c r="E51" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -2066,8 +2583,11 @@
       <c r="E52" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>44</v>
       </c>
@@ -2083,8 +2603,11 @@
       <c r="E53" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>45</v>
       </c>
@@ -2100,8 +2623,11 @@
       <c r="E54" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -2117,8 +2643,11 @@
       <c r="E55" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -2134,8 +2663,11 @@
       <c r="E56" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -2151,8 +2683,11 @@
       <c r="E57" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -2168,8 +2703,11 @@
       <c r="E58" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -2185,8 +2723,11 @@
       <c r="E59" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>51</v>
       </c>
@@ -2202,8 +2743,11 @@
       <c r="E60" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>52</v>
       </c>
@@ -2219,8 +2763,11 @@
       <c r="E61" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -2236,8 +2783,11 @@
       <c r="E62" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>54</v>
       </c>
@@ -2253,8 +2803,11 @@
       <c r="E63" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -2270,8 +2823,11 @@
       <c r="E64" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -2287,8 +2843,11 @@
       <c r="E65" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>57</v>
       </c>
@@ -2304,8 +2863,11 @@
       <c r="E66" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -2321,8 +2883,11 @@
       <c r="E67" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -2338,8 +2903,11 @@
       <c r="E68" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -2355,8 +2923,11 @@
       <c r="E69" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>61</v>
       </c>
@@ -2372,8 +2943,11 @@
       <c r="E70" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>62</v>
       </c>
@@ -2389,8 +2963,11 @@
       <c r="E71" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -2406,8 +2983,11 @@
       <c r="E72" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>64</v>
       </c>
@@ -2423,8 +3003,11 @@
       <c r="E73" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>65</v>
       </c>
@@ -2440,8 +3023,11 @@
       <c r="E74" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>66</v>
       </c>
@@ -2457,8 +3043,11 @@
       <c r="E75" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -2474,8 +3063,11 @@
       <c r="E76" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>68</v>
       </c>
@@ -2491,8 +3083,11 @@
       <c r="E77" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>69</v>
       </c>
@@ -2508,8 +3103,11 @@
       <c r="E78" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>70</v>
       </c>
@@ -2525,8 +3123,11 @@
       <c r="E79" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>71</v>
       </c>
@@ -2542,8 +3143,11 @@
       <c r="E80" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>72</v>
       </c>
@@ -2559,8 +3163,11 @@
       <c r="E81" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>73</v>
       </c>
@@ -2576,8 +3183,11 @@
       <c r="E82" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>74</v>
       </c>
@@ -2593,8 +3203,11 @@
       <c r="E83" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>75</v>
       </c>
@@ -2610,8 +3223,11 @@
       <c r="E84" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>76</v>
       </c>
@@ -2627,8 +3243,11 @@
       <c r="E85" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>77</v>
       </c>
@@ -2644,8 +3263,11 @@
       <c r="E86" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>78</v>
       </c>
@@ -2661,8 +3283,11 @@
       <c r="E87" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>79</v>
       </c>
@@ -2678,8 +3303,11 @@
       <c r="E88" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>80</v>
       </c>
@@ -2695,8 +3323,11 @@
       <c r="E89" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>81</v>
       </c>
@@ -2712,8 +3343,11 @@
       <c r="E90" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>82</v>
       </c>
@@ -2729,8 +3363,11 @@
       <c r="E91" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>83</v>
       </c>
@@ -2746,8 +3383,11 @@
       <c r="E92" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>84</v>
       </c>
@@ -2763,8 +3403,11 @@
       <c r="E93" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>85</v>
       </c>
@@ -2780,8 +3423,11 @@
       <c r="E94" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>86</v>
       </c>
@@ -2797,8 +3443,11 @@
       <c r="E95" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>87</v>
       </c>
@@ -2814,8 +3463,11 @@
       <c r="E96" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>88</v>
       </c>
@@ -2831,8 +3483,11 @@
       <c r="E97" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>89</v>
       </c>
@@ -2848,8 +3503,11 @@
       <c r="E98" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>90</v>
       </c>
@@ -2865,8 +3523,11 @@
       <c r="E99" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>91</v>
       </c>
@@ -2882,8 +3543,11 @@
       <c r="E100" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>92</v>
       </c>
@@ -2899,8 +3563,11 @@
       <c r="E101" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>93</v>
       </c>
@@ -2916,8 +3583,11 @@
       <c r="E102" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>94</v>
       </c>
@@ -2933,8 +3603,11 @@
       <c r="E103" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F103" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>95</v>
       </c>
@@ -2950,8 +3623,11 @@
       <c r="E104" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F104" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>96</v>
       </c>
@@ -2967,8 +3643,11 @@
       <c r="E105" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F105" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>97</v>
       </c>
@@ -2984,8 +3663,11 @@
       <c r="E106" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F106" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>98</v>
       </c>
@@ -3001,8 +3683,11 @@
       <c r="E107" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F107" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>99</v>
       </c>
@@ -3018,8 +3703,11 @@
       <c r="E108" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F108" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>100</v>
       </c>
@@ -3035,8 +3723,11 @@
       <c r="E109" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F109" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>101</v>
       </c>
@@ -3052,8 +3743,11 @@
       <c r="E110" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F110" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>102</v>
       </c>
@@ -3069,8 +3763,11 @@
       <c r="E111" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F111" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>103</v>
       </c>
@@ -3086,8 +3783,11 @@
       <c r="E112" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F112" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>104</v>
       </c>
@@ -3103,8 +3803,11 @@
       <c r="E113" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F113" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>105</v>
       </c>
@@ -3120,8 +3823,11 @@
       <c r="E114" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F114" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>106</v>
       </c>
@@ -3137,8 +3843,11 @@
       <c r="E115" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F115" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>107</v>
       </c>
@@ -3154,8 +3863,11 @@
       <c r="E116" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F116" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>108</v>
       </c>
@@ -3171,8 +3883,11 @@
       <c r="E117" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F117" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>109</v>
       </c>
@@ -3188,8 +3903,11 @@
       <c r="E118" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F118" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>110</v>
       </c>
@@ -3205,8 +3923,11 @@
       <c r="E119" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F119" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>111</v>
       </c>
@@ -3222,8 +3943,11 @@
       <c r="E120" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F120" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>112</v>
       </c>
@@ -3239,8 +3963,11 @@
       <c r="E121" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F121" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>113</v>
       </c>
@@ -3255,11 +3982,15 @@
       </c>
       <c r="E122" t="s">
         <v>139</v>
+      </c>
+      <c r="F122" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7162,7 +7893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11AFBC05-20B7-4C67-B971-1B13AF228B2C}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: add citta combination table
</commit_message>
<xml_diff>
--- a/documents/Sheet.xlsx
+++ b/documents/Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jordi\Home\20_Areas\10_Dhammobhasa\dhammo-konvajs\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45E4847-B20D-44A3-A70C-AA3B39E607AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A01B40-952E-41D2-9B9B-320C5F92D248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Citta" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,12 @@
     <sheet name="Cetasika layout" sheetId="4" r:id="rId4"/>
     <sheet name="Cittuppada" sheetId="5" r:id="rId5"/>
     <sheet name="Cetasika groups" sheetId="6" r:id="rId6"/>
+    <sheet name="Combination" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="CetasikaID">Cetasika!$A$2:$A$53</definedName>
+    <definedName name="CittaID">Citta!$A$2:$A$122</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="382">
   <si>
     <t>id</t>
   </si>
@@ -1173,6 +1178,9 @@
   </si>
   <si>
     <t>nevasaññānāsaññāyatana kiriya citta</t>
+  </si>
+  <si>
+    <t>cetasika/0</t>
   </si>
 </sst>
 </file>
@@ -1534,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30282B-4D63-4407-A836-371A28DA1D49}">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A102" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5721,8 +5729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DC72FF-BEDA-4115-96FD-61449208A603}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A47"/>
+    <sheetView topLeftCell="A42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A53" sqref="A2:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8123,4 +8131,734 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33340F1D-74D4-4958-9F44-1892C276E953}">
+  <dimension ref="A1:D93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="106" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>40</v>
+      </c>
+      <c r="B74" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>43</v>
+      </c>
+      <c r="B83" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>44</v>
+      </c>
+      <c r="B86" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>44</v>
+      </c>
+      <c r="B87" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>45</v>
+      </c>
+      <c r="B90" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>46</v>
+      </c>
+      <c r="B92" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A100" xr:uid="{25956C15-9A59-44C2-BA60-488C5603ECF8}">
+      <formula1>CittaID</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F21 B18:D21 B2:F17 C22:F40 B22:B93" xr:uid="{F97112C0-7299-4848-9D80-4621B27E7192}">
+      <formula1>CetasikaID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: citta combination citta panel
</commit_message>
<xml_diff>
--- a/documents/Sheet.xlsx
+++ b/documents/Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jordi\Home\20_Areas\10_Dhammobhasa\dhammo-konvajs\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A01B40-952E-41D2-9B9B-320C5F92D248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AADEF6-E85E-4EB2-BFDA-CC3AD1135617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="382">
   <si>
     <t>id</t>
   </si>
@@ -8135,10 +8135,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33340F1D-74D4-4958-9F44-1892C276E953}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="106" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8185,25 +8185,37 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>161</v>
       </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>161</v>
@@ -8211,41 +8223,50 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>165</v>
+      </c>
+      <c r="C12" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>161</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>162</v>
@@ -8253,7 +8274,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>163</v>
@@ -8261,7 +8282,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>164</v>
@@ -8271,24 +8292,12 @@
       <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C18" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -8297,12 +8306,6 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" t="s">
-        <v>166</v>
-      </c>
-      <c r="D20" t="s">
         <v>163</v>
       </c>
     </row>
@@ -8311,551 +8314,598 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
-      </c>
-      <c r="C21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D21" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>187</v>
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>188</v>
+        <v>165</v>
+      </c>
+      <c r="C24" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>189</v>
+        <v>165</v>
+      </c>
+      <c r="C25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B32" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
-      <c r="B38" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>26</v>
       </c>
-      <c r="B44" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B46" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>27</v>
       </c>
-      <c r="B50" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B52" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>28</v>
       </c>
-      <c r="B56" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B58" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B61" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>29</v>
       </c>
-      <c r="B62" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B64" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>30</v>
       </c>
-      <c r="B68" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>30</v>
       </c>
       <c r="B69" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="B70" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="B73" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>40</v>
-      </c>
-      <c r="B74" t="s">
-        <v>190</v>
+        <v>39</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B75" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="B76" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>41</v>
-      </c>
-      <c r="B77" t="s">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B78" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B79" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>42</v>
-      </c>
-      <c r="B80" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="B82" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>43</v>
-      </c>
-      <c r="B83" t="s">
-        <v>190</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="B85" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>44</v>
-      </c>
-      <c r="B86" t="s">
-        <v>190</v>
+        <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B88" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>45</v>
-      </c>
-      <c r="B89" t="s">
-        <v>190</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B90" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B91" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>46</v>
-      </c>
-      <c r="B92" t="s">
-        <v>190</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>45</v>
+      </c>
+      <c r="B93" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>46</v>
       </c>
-      <c r="B93" t="s">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>46</v>
+      </c>
+      <c r="B96" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>46</v>
+      </c>
+      <c r="B97" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A100" xr:uid="{25956C15-9A59-44C2-BA60-488C5603ECF8}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F22:F25 B22:D25 B26:B97 C26:F44 B2:F21" xr:uid="{F97112C0-7299-4848-9D80-4621B27E7192}">
+      <formula1>CetasikaID</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A104" xr:uid="{25956C15-9A59-44C2-BA60-488C5603ECF8}">
       <formula1>CittaID</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F21 B18:D21 B2:F17 C22:F40 B22:B93" xr:uid="{F97112C0-7299-4848-9D80-4621B27E7192}">
-      <formula1>CetasikaID</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: fix combination table
</commit_message>
<xml_diff>
--- a/documents/Sheet.xlsx
+++ b/documents/Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jordi\Home\20_Areas\10_Dhammobhasa\dhammo-konvajs\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AADEF6-E85E-4EB2-BFDA-CC3AD1135617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC4BE65-4D6E-4656-803B-F304A44082CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{6BEDAB92-91DE-46F1-9E2F-02163BE0E66F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="382">
   <si>
     <t>id</t>
   </si>
@@ -8135,10 +8135,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33340F1D-74D4-4958-9F44-1892C276E953}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A133" sqref="A1:D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8898,10 +8898,262 @@
         <v>191</v>
       </c>
     </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>47</v>
+      </c>
+      <c r="B99" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>47</v>
+      </c>
+      <c r="B100" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>48</v>
+      </c>
+      <c r="B102" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>48</v>
+      </c>
+      <c r="B103" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>49</v>
+      </c>
+      <c r="B105" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>49</v>
+      </c>
+      <c r="B106" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>50</v>
+      </c>
+      <c r="B108" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>50</v>
+      </c>
+      <c r="B109" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>52</v>
+      </c>
+      <c r="B111" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>52</v>
+      </c>
+      <c r="B112" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>53</v>
+      </c>
+      <c r="B114" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>53</v>
+      </c>
+      <c r="B115" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>54</v>
+      </c>
+      <c r="B117" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>54</v>
+      </c>
+      <c r="B118" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>55</v>
+      </c>
+      <c r="B120" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>55</v>
+      </c>
+      <c r="B121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>57</v>
+      </c>
+      <c r="B123" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>57</v>
+      </c>
+      <c r="B124" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>58</v>
+      </c>
+      <c r="B126" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>58</v>
+      </c>
+      <c r="B127" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>59</v>
+      </c>
+      <c r="B129" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>59</v>
+      </c>
+      <c r="B130" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>60</v>
+      </c>
+      <c r="B132" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>60</v>
+      </c>
+      <c r="B133" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F22:F25 B22:D25 B26:B97 C26:F44 B2:F21" xr:uid="{F97112C0-7299-4848-9D80-4621B27E7192}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F22:F25 B22:D25 B26:B133 C26:F44 B2:F21" xr:uid="{F97112C0-7299-4848-9D80-4621B27E7192}">
       <formula1>CetasikaID</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A104" xr:uid="{25956C15-9A59-44C2-BA60-488C5603ECF8}">

</xml_diff>